<commit_message>
Improvement on popup window handling
</commit_message>
<xml_diff>
--- a/Software/Packages/Resources/Project_Information.xlsx
+++ b/Software/Packages/Resources/Project_Information.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="SMT" sheetId="3" r:id="rId2"/>
-    <sheet name="SWT" sheetId="2" r:id="rId3"/>
-    <sheet name="SWIT" sheetId="7" r:id="rId4"/>
-    <sheet name="PROJECT_CONFIG" sheetId="4" r:id="rId5"/>
-    <sheet name="TEST_CONFIG" sheetId="5" r:id="rId6"/>
-    <sheet name="TEST_ENV_CONFIG" sheetId="6" r:id="rId7"/>
+    <sheet name="Test_Cases" sheetId="8" r:id="rId3"/>
+    <sheet name="PROJECT_CONFIG" sheetId="4" r:id="rId4"/>
+    <sheet name="TEST_CONFIG" sheetId="5" r:id="rId5"/>
+    <sheet name="TEST_ENV_CONFIG" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>DRV</t>
   </si>
@@ -83,6 +82,42 @@
   </si>
   <si>
     <t>_789</t>
+  </si>
+  <si>
+    <t>HSIT</t>
+  </si>
+  <si>
+    <t>RRST</t>
+  </si>
+  <si>
+    <t>p_Test_Env_Cfg</t>
+  </si>
+  <si>
+    <t>OSCILLOSCOPE</t>
+  </si>
+  <si>
+    <t>LOGIC_ANALYZER</t>
+  </si>
+  <si>
+    <t>POWER_SUPPLY</t>
+  </si>
+  <si>
+    <t>tc_ID</t>
+  </si>
+  <si>
+    <t>tc_COMMAND</t>
+  </si>
+  <si>
+    <t>tc_FUNCTIONALITY</t>
+  </si>
+  <si>
+    <t>tc_VARIANT</t>
+  </si>
+  <si>
+    <t>tc_CARLINE</t>
+  </si>
+  <si>
+    <t>tc_POSITION</t>
   </si>
 </sst>
 </file>
@@ -444,35 +479,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -562,49 +613,87 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>